<commit_message>
covered date/time functions: determined job posting per hour
</commit_message>
<xml_diff>
--- a/0_Resources/Problems/2_Formulas_Functions/9_Date_Time_Functions.xlsx
+++ b/0_Resources/Problems/2_Formulas_Functions/9_Date_Time_Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Okoko\Desktop\DATA ANALYSIS PROJECT\EXCEL PROJECTS\excel_data_analytics_project\0_Resources\Problems\2_Formulas_Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C08F6B-577E-40FC-87A2-A00B849E81C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7616DE58-6746-44AA-8A15-C36632B3800C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18336" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
@@ -38,6 +38,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,6 +615,433 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Job</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> posting per hour</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$AA$2:$AA$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$AB$2:$AB$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C072-4E91-A13D-DD580602E2B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="628336136"/>
+        <c:axId val="628333616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="628336136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628333616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="628333616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="628336136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
               <a:t>Application</a:t>
             </a:r>
             <a:r>
@@ -1055,6 +1504,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1597,7 +2086,551 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E92D9707-73C7-3745-FA84-807DA52D743C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1901,32 +2934,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5E7F13-C613-4452-9CDB-2C26D6876D9D}">
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AC18" sqref="AC18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.578125" customWidth="1"/>
-    <col min="2" max="2" width="14.26171875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="27.26171875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.26171875" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="10" max="13" width="8.83984375" customWidth="1"/>
-    <col min="14" max="14" width="14.20703125" customWidth="1"/>
-    <col min="15" max="17" width="8.83984375" customWidth="1"/>
-    <col min="18" max="18" width="15.9453125" customWidth="1"/>
-    <col min="19" max="23" width="8.83984375" customWidth="1"/>
-    <col min="24" max="25" width="14.3671875" customWidth="1"/>
-    <col min="26" max="26" width="8.83984375" customWidth="1"/>
+    <col min="10" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="19" max="23" width="8.85546875" customWidth="1"/>
+    <col min="24" max="25" width="14.42578125" customWidth="1"/>
+    <col min="26" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -1990,7 +3025,7 @@
       </c>
       <c r="AB1" s="16"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -2015,11 +3050,64 @@
       <c r="H2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="X2" s="13"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J2">
+        <f>MONTH(D2)</f>
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <f>DAY(D2)</f>
+        <v>14</v>
+      </c>
+      <c r="L2">
+        <f>YEAR(D2)</f>
+        <v>2023</v>
+      </c>
+      <c r="N2" s="9">
+        <f>DATE(L2,J2,K2)</f>
+        <v>44971</v>
+      </c>
+      <c r="P2" s="9">
+        <f ca="1">TODAY()</f>
+        <v>45921</v>
+      </c>
+      <c r="R2">
+        <f ca="1">DATEDIF(N2,P2,"Y")</f>
+        <v>2</v>
+      </c>
+      <c r="T2">
+        <f>HOUR(D2)</f>
+        <v>15</v>
+      </c>
+      <c r="U2">
+        <f>MINUTE(D2)</f>
+        <v>22</v>
+      </c>
+      <c r="V2">
+        <f>SECOND(D2)</f>
+        <v>15</v>
+      </c>
+      <c r="X2" s="13">
+        <f>TIME(T2,U2,V2)</f>
+        <v>0.64045138888888886</v>
+      </c>
+      <c r="Y2" t="str">
+        <f>TEXT(D2,"HH:MM AM/PM")</f>
+        <v>03:22 PM</v>
+      </c>
+      <c r="Z2" cm="1">
+        <f t="array" ref="Z2:Z21">HOUR(Y2:Y21)</f>
+        <v>15</v>
+      </c>
+      <c r="AA2" cm="1">
+        <f t="array" ref="AA2:AA25">_xlfn.SEQUENCE(24,,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <f>COUNTIF(_xlfn.ANCHORARRAY($Z$2),AA2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -2044,10 +3132,62 @@
       <c r="H3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="9"/>
-      <c r="X3" s="13"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J3">
+        <f t="shared" ref="J3:J21" si="0">MONTH(D3)</f>
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K21" si="1">DAY(D3)</f>
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L21" si="2">YEAR(D3)</f>
+        <v>2023</v>
+      </c>
+      <c r="N3" s="9">
+        <f t="shared" ref="N3:N21" si="3">DATE(L3,J3,K3)</f>
+        <v>45055</v>
+      </c>
+      <c r="P3" s="9">
+        <f t="shared" ref="P3:P22" ca="1" si="4">TODAY()</f>
+        <v>45921</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R20" ca="1" si="5">DATEDIF(N3,P3,"Y")</f>
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T20" si="6">HOUR(D3)</f>
+        <v>9</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U20" si="7">MINUTE(D3)</f>
+        <v>45</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V20" si="8">SECOND(D3)</f>
+        <v>32</v>
+      </c>
+      <c r="X3" s="13">
+        <f t="shared" ref="X3:X21" si="9">TIME(T3,U3,V3)</f>
+        <v>0.40662037037037035</v>
+      </c>
+      <c r="Y3" t="str">
+        <f t="shared" ref="Y3:Y21" si="10">TEXT(D3,"HH:MM AM/PM")</f>
+        <v>09:45 AM</v>
+      </c>
+      <c r="Z3">
+        <v>9</v>
+      </c>
+      <c r="AA3">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB25" si="11">COUNTIF(_xlfn.ANCHORARRAY($Z$2),AA3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2072,10 +3212,62 @@
       <c r="H4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="X4" s="13"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="N4" s="9">
+        <f t="shared" si="3"/>
+        <v>45128</v>
+      </c>
+      <c r="P4" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="X4" s="13">
+        <f t="shared" si="9"/>
+        <v>0.72971064814814812</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="10"/>
+        <v>05:30 PM</v>
+      </c>
+      <c r="Z4">
+        <v>17</v>
+      </c>
+      <c r="AA4">
+        <v>3</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -2100,10 +3292,62 @@
       <c r="H5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="9"/>
-      <c r="X5" s="13"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="N5" s="9">
+        <f t="shared" si="3"/>
+        <v>45173</v>
+      </c>
+      <c r="P5" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="X5" s="13">
+        <f t="shared" si="9"/>
+        <v>0.3021875</v>
+      </c>
+      <c r="Y5" t="str">
+        <f t="shared" si="10"/>
+        <v>07:15 AM</v>
+      </c>
+      <c r="Z5">
+        <v>7</v>
+      </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -2128,10 +3372,62 @@
       <c r="H6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="X6" s="13"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="N6" s="9">
+        <f t="shared" si="3"/>
+        <v>45248</v>
+      </c>
+      <c r="P6" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+      <c r="X6" s="13">
+        <f t="shared" si="9"/>
+        <v>0.70857638888888885</v>
+      </c>
+      <c r="Y6" t="str">
+        <f t="shared" si="10"/>
+        <v>05:00 PM</v>
+      </c>
+      <c r="Z6">
+        <v>17</v>
+      </c>
+      <c r="AA6">
+        <v>5</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -2156,10 +3452,62 @@
       <c r="H7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="9"/>
-      <c r="X7" s="13"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N7" s="9">
+        <f t="shared" si="3"/>
+        <v>45302</v>
+      </c>
+      <c r="P7" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="8"/>
+        <v>58</v>
+      </c>
+      <c r="X7" s="13">
+        <f t="shared" si="9"/>
+        <v>0.53192129629629625</v>
+      </c>
+      <c r="Y7" t="str">
+        <f t="shared" si="10"/>
+        <v>12:45 PM</v>
+      </c>
+      <c r="Z7">
+        <v>12</v>
+      </c>
+      <c r="AA7">
+        <v>6</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
@@ -2184,10 +3532,62 @@
       <c r="H8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="X8" s="13"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N8" s="9">
+        <f t="shared" si="3"/>
+        <v>45354</v>
+      </c>
+      <c r="P8" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="8"/>
+        <v>33</v>
+      </c>
+      <c r="X8" s="13">
+        <f t="shared" si="9"/>
+        <v>0.68788194444444439</v>
+      </c>
+      <c r="Y8" t="str">
+        <f t="shared" si="10"/>
+        <v>04:30 PM</v>
+      </c>
+      <c r="Z8">
+        <v>16</v>
+      </c>
+      <c r="AA8">
+        <v>7</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -2212,10 +3612,62 @@
       <c r="H9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="9"/>
-      <c r="X9" s="13"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N9" s="9">
+        <f t="shared" si="3"/>
+        <v>45408</v>
+      </c>
+      <c r="P9" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="8"/>
+        <v>46</v>
+      </c>
+      <c r="X9" s="13">
+        <f t="shared" si="9"/>
+        <v>0.34081018518518519</v>
+      </c>
+      <c r="Y9" t="str">
+        <f t="shared" si="10"/>
+        <v>08:10 AM</v>
+      </c>
+      <c r="Z9">
+        <v>8</v>
+      </c>
+      <c r="AA9">
+        <v>8</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -2240,10 +3692,62 @@
       <c r="H10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="9"/>
-      <c r="X10" s="13"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N10" s="9">
+        <f t="shared" si="3"/>
+        <v>45458</v>
+      </c>
+      <c r="P10" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="X10" s="13">
+        <f t="shared" si="9"/>
+        <v>0.74333333333333329</v>
+      </c>
+      <c r="Y10" t="str">
+        <f t="shared" si="10"/>
+        <v>05:50 PM</v>
+      </c>
+      <c r="Z10">
+        <v>17</v>
+      </c>
+      <c r="AA10">
+        <v>9</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -2268,10 +3772,62 @@
       <c r="H11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="9"/>
-      <c r="X11" s="13"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N11" s="9">
+        <f t="shared" si="3"/>
+        <v>45480</v>
+      </c>
+      <c r="P11" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R11">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="8"/>
+        <v>36</v>
+      </c>
+      <c r="X11" s="13">
+        <f t="shared" si="9"/>
+        <v>0.60805555555555557</v>
+      </c>
+      <c r="Y11" t="str">
+        <f t="shared" si="10"/>
+        <v>02:35 PM</v>
+      </c>
+      <c r="Z11">
+        <v>14</v>
+      </c>
+      <c r="AA11">
+        <v>10</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
@@ -2296,10 +3852,62 @@
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="9"/>
-      <c r="X12" s="13"/>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N12" s="9">
+        <f t="shared" si="3"/>
+        <v>45455</v>
+      </c>
+      <c r="P12" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="X12" s="13">
+        <f t="shared" si="9"/>
+        <v>0.28493055555555558</v>
+      </c>
+      <c r="Y12" t="str">
+        <f t="shared" si="10"/>
+        <v>06:50 AM</v>
+      </c>
+      <c r="Z12">
+        <v>6</v>
+      </c>
+      <c r="AA12">
+        <v>11</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -2324,10 +3932,62 @@
       <c r="H13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N13" s="9"/>
-      <c r="X13" s="13"/>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="N13" s="9">
+        <f t="shared" si="3"/>
+        <v>44951</v>
+      </c>
+      <c r="P13" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R13">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="X13" s="13">
+        <f t="shared" si="9"/>
+        <v>0.55214120370370368</v>
+      </c>
+      <c r="Y13" t="str">
+        <f t="shared" si="10"/>
+        <v>01:15 PM</v>
+      </c>
+      <c r="Z13">
+        <v>13</v>
+      </c>
+      <c r="AA13">
+        <v>12</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -2352,10 +4012,62 @@
       <c r="H14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="9"/>
-      <c r="X14" s="13"/>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="N14" s="9">
+        <f t="shared" si="3"/>
+        <v>45002</v>
+      </c>
+      <c r="P14" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="7"/>
+        <v>45</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+      <c r="X14" s="13">
+        <f t="shared" si="9"/>
+        <v>0.49003472222222222</v>
+      </c>
+      <c r="Y14" t="str">
+        <f t="shared" si="10"/>
+        <v>11:45 AM</v>
+      </c>
+      <c r="Z14">
+        <v>11</v>
+      </c>
+      <c r="AA14">
+        <v>13</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -2380,10 +4092,62 @@
       <c r="H15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="9"/>
-      <c r="X15" s="13"/>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.55000000000000004">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="N15" s="9">
+        <f t="shared" si="3"/>
+        <v>45078</v>
+      </c>
+      <c r="P15" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R15">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="8"/>
+        <v>51</v>
+      </c>
+      <c r="X15" s="13">
+        <f t="shared" si="9"/>
+        <v>0.41725694444444444</v>
+      </c>
+      <c r="Y15" t="str">
+        <f t="shared" si="10"/>
+        <v>10:00 AM</v>
+      </c>
+      <c r="Z15">
+        <v>10</v>
+      </c>
+      <c r="AA15">
+        <v>14</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
@@ -2408,10 +4172,62 @@
       <c r="H16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N16" s="9"/>
-      <c r="X16" s="13"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="N16" s="9">
+        <f t="shared" si="3"/>
+        <v>45168</v>
+      </c>
+      <c r="P16" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="X16" s="13">
+        <f t="shared" si="9"/>
+        <v>0.72932870370370373</v>
+      </c>
+      <c r="Y16" t="str">
+        <f t="shared" si="10"/>
+        <v>05:30 PM</v>
+      </c>
+      <c r="Z16">
+        <v>17</v>
+      </c>
+      <c r="AA16">
+        <v>15</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -2436,10 +4252,62 @@
       <c r="H17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N17" s="9"/>
-      <c r="X17" s="13"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>2023</v>
+      </c>
+      <c r="N17" s="9">
+        <f t="shared" si="3"/>
+        <v>45218</v>
+      </c>
+      <c r="P17" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R17">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="X17" s="13">
+        <f t="shared" si="9"/>
+        <v>0.3197800925925926</v>
+      </c>
+      <c r="Y17" t="str">
+        <f t="shared" si="10"/>
+        <v>07:40 AM</v>
+      </c>
+      <c r="Z17">
+        <v>7</v>
+      </c>
+      <c r="AA17">
+        <v>16</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -2464,10 +4332,62 @@
       <c r="H18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="9"/>
-      <c r="X18" s="13"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N18" s="9">
+        <f t="shared" si="3"/>
+        <v>45350</v>
+      </c>
+      <c r="P18" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R18">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="8"/>
+        <v>42</v>
+      </c>
+      <c r="X18" s="13">
+        <f t="shared" si="9"/>
+        <v>0.71923611111111108</v>
+      </c>
+      <c r="Y18" t="str">
+        <f t="shared" si="10"/>
+        <v>05:15 PM</v>
+      </c>
+      <c r="Z18">
+        <v>17</v>
+      </c>
+      <c r="AA18">
+        <v>17</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
@@ -2492,10 +4412,62 @@
       <c r="H19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N19" s="9"/>
-      <c r="X19" s="13"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N19" s="9">
+        <f t="shared" si="3"/>
+        <v>45418</v>
+      </c>
+      <c r="P19" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R19">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="7"/>
+        <v>25</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="8"/>
+        <v>57</v>
+      </c>
+      <c r="X19" s="13">
+        <f t="shared" si="9"/>
+        <v>0.72635416666666663</v>
+      </c>
+      <c r="Y19" t="str">
+        <f t="shared" si="10"/>
+        <v>05:25 PM</v>
+      </c>
+      <c r="Z19">
+        <v>17</v>
+      </c>
+      <c r="AA19">
+        <v>18</v>
+      </c>
+      <c r="AB19">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -2520,10 +4492,62 @@
       <c r="H20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N20" s="9"/>
-      <c r="X20" s="13"/>
-    </row>
-    <row r="21" spans="1:24" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N20" s="9">
+        <f t="shared" si="3"/>
+        <v>45496</v>
+      </c>
+      <c r="P20" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R20">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="X20" s="13">
+        <f t="shared" si="9"/>
+        <v>0.29170138888888891</v>
+      </c>
+      <c r="Y20" t="str">
+        <f t="shared" si="10"/>
+        <v>07:00 AM</v>
+      </c>
+      <c r="Z20">
+        <v>7</v>
+      </c>
+      <c r="AA20">
+        <v>19</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -2548,8 +4572,97 @@
       <c r="H21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N21" s="9"/>
-      <c r="X21" s="13"/>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>2024</v>
+      </c>
+      <c r="N21" s="9">
+        <f t="shared" si="3"/>
+        <v>45422</v>
+      </c>
+      <c r="P21" s="9">
+        <f t="shared" ca="1" si="4"/>
+        <v>45921</v>
+      </c>
+      <c r="R21">
+        <f ca="1">DATEDIF(N21,P21,"Y")</f>
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <f>HOUR(D21)</f>
+        <v>17</v>
+      </c>
+      <c r="U21">
+        <f>MINUTE(D21)</f>
+        <v>45</v>
+      </c>
+      <c r="V21">
+        <f>SECOND(D21)</f>
+        <v>26</v>
+      </c>
+      <c r="X21" s="13">
+        <f t="shared" si="9"/>
+        <v>0.73988425925925927</v>
+      </c>
+      <c r="Y21" t="str">
+        <f t="shared" si="10"/>
+        <v>05:45 PM</v>
+      </c>
+      <c r="Z21">
+        <v>17</v>
+      </c>
+      <c r="AA21">
+        <v>20</v>
+      </c>
+      <c r="AB21">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="P22" s="9"/>
+      <c r="AA22">
+        <v>21</v>
+      </c>
+      <c r="AB22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA23">
+        <v>22</v>
+      </c>
+      <c r="AB23">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA24">
+        <v>23</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA25">
+        <v>24</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H22">
@@ -2557,6 +4670,7 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2568,23 +4682,23 @@
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="29.83984375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="22" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="40" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="1.83984375" customWidth="1"/>
-    <col min="14" max="14" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -2628,7 +4742,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -2671,14 +4785,14 @@
       </c>
       <c r="P2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45538</v>
+        <v>45921</v>
       </c>
       <c r="R2">
         <f ca="1">DATEDIF(D2,$P$2,"D")</f>
-        <v>567</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -2721,10 +4835,10 @@
       </c>
       <c r="R3">
         <f ca="1">DATEDIF(D3,$P$2,"D")</f>
-        <v>483</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2767,10 +4881,10 @@
       </c>
       <c r="R4">
         <f t="shared" ref="R4:R21" ca="1" si="4">DATEDIF(D4,$P$2,"D")</f>
-        <v>410</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -2813,10 +4927,10 @@
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="4"/>
-        <v>365</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -2859,10 +4973,10 @@
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="4"/>
-        <v>290</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -2905,10 +5019,10 @@
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="4"/>
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
@@ -2952,10 +5066,10 @@
       <c r="P8" s="9"/>
       <c r="R8">
         <f t="shared" ca="1" si="4"/>
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -2998,10 +5112,10 @@
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="4"/>
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -3044,10 +5158,10 @@
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="4"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -3090,10 +5204,10 @@
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="4"/>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
@@ -3136,10 +5250,10 @@
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="4"/>
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -3182,10 +5296,10 @@
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="4"/>
-        <v>587</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -3228,10 +5342,10 @@
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="4"/>
-        <v>536</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -3274,10 +5388,10 @@
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="4"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
@@ -3320,10 +5434,10 @@
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="4"/>
-        <v>370</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -3366,10 +5480,10 @@
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="4"/>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -3412,10 +5526,10 @@
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="4"/>
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
@@ -3458,10 +5572,10 @@
       </c>
       <c r="R19">
         <f t="shared" ca="1" si="4"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -3504,10 +5618,10 @@
       </c>
       <c r="R20">
         <f t="shared" ca="1" si="4"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -3550,7 +5664,7 @@
       </c>
       <c r="R21">
         <f t="shared" ca="1" si="4"/>
-        <v>116</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -3566,22 +5680,22 @@
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="29.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.734375" customWidth="1"/>
-    <col min="14" max="14" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.41796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>63</v>
       </c>
@@ -3626,7 +5740,7 @@
       </c>
       <c r="R1" s="16"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
@@ -3678,7 +5792,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -3731,7 +5845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -3784,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -3837,7 +5951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>68</v>
       </c>
@@ -3890,7 +6004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>69</v>
       </c>
@@ -3943,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>70</v>
       </c>
@@ -3996,7 +6110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>71</v>
       </c>
@@ -4049,7 +6163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>72</v>
       </c>
@@ -4102,7 +6216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>73</v>
       </c>
@@ -4155,7 +6269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>74</v>
       </c>
@@ -4208,7 +6322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>75</v>
       </c>
@@ -4261,7 +6375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>76</v>
       </c>
@@ -4314,7 +6428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>77</v>
       </c>
@@ -4367,7 +6481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>78</v>
       </c>
@@ -4420,7 +6534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
@@ -4473,7 +6587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>80</v>
       </c>
@@ -4526,7 +6640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>81</v>
       </c>
@@ -4579,7 +6693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -4632,7 +6746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>83</v>
       </c>
@@ -4685,7 +6799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q22" s="14">
         <v>20</v>
       </c>
@@ -4694,7 +6808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q23" s="14">
         <v>21</v>
       </c>
@@ -4703,7 +6817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q24" s="14">
         <v>22</v>
       </c>
@@ -4712,7 +6826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q25" s="14">
         <v>23</v>
       </c>
@@ -4721,7 +6835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="Q26" s="14">
         <v>24</v>
       </c>

</xml_diff>